<commit_message>
feat: test UI results
</commit_message>
<xml_diff>
--- a/таблица результатов.xlsx
+++ b/таблица результатов.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\! Аспирантура\статья\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerumi\10. Информатика\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931C8692-444A-4772-BA40-FC9FEF5D2035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30470D6-C673-4D5F-B198-80F01216D6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,146 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Zerumi</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{DCA5197E-F487-455B-9DE5-BC574F395602}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Zerumi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+время в результатах измеряется в секундах</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{E224B44E-B847-4C40-9488-45B7D2999CAE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Zerumi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+14.05.23 6:21 -- найти с помощью фильтра по событям 3.06 нужное мероприятие не удалось.
+Затрачено времени: 59.2с</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{A8B60C99-7274-4A09-ABCA-4E82859D783C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zerumi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+14.05.2023 4:55 -- сайт не работает: 504 Gateaway timeout</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{A228C729-C2C7-4058-8EFF-E595817F7910}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Zerumi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+14.05.2023 5:27 -- ни одного телефона Apple не было в продаже, и как следствие, они не отображались в поиске.
+Затрачено времени: 43,3с</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{F9D4994A-51E4-4242-AFE2-5E41BB014C60}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Zerumi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+14.05.2023 5:30 -- За ~30 минут простоя вкладки успела упасть кнопка "Каталог", пришлось перезагружать сайт</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
@@ -124,7 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +296,34 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -474,11 +642,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,16 +680,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>513</v>
+        <v>39.29</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>213</v>
+        <v>15.83</v>
       </c>
       <c r="E2">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -529,16 +697,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>513</v>
+        <v>48.14</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>213</v>
+        <v>14.69</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -546,16 +714,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>513</v>
+        <v>42.52</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>213</v>
+        <v>11.54</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -563,16 +731,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>513</v>
+        <v>30.47</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>213</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,31 +767,103 @@
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>27.86</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>21.29</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>25.09</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>15.46</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>20.27</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>22.77</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>15.21</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>10.24</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -646,36 +886,120 @@
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="B17">
+        <v>49.31</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>17.329999999999998</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>16.09</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>26.1</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="B19">
+        <v>25.4</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>10.67</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="B21">
+        <v>34.54</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>20.12</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B22">
+        <v>27.31</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>9.82</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B23">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>13.12</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -698,35 +1022,119 @@
       <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B27">
+        <v>26.62</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>9.35</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B28">
+        <v>20.02</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="B29">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>10.56</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="B30">
+        <v>14.42</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>11.37</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="B31">
+        <v>23.74</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>76.2</v>
+      </c>
+      <c r="C32">
+        <v>9</v>
+      </c>
+      <c r="D32">
+        <v>12.33</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="B33">
+        <v>41.33</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>9.9</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -758,5 +1166,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
+  <legacyDrawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>